<commit_message>
Actualizacion 2 - Semana 6
</commit_message>
<xml_diff>
--- a/DatosAgroNet_limpio.xlsx
+++ b/DatosAgroNet_limpio.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B133"/>
+  <dimension ref="A1:B82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,1057 +451,649 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44928</v>
+        <v>45292</v>
       </c>
       <c r="B2" t="n">
-        <v>10095</v>
+        <v>14271.7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44935</v>
+        <v>45299</v>
       </c>
       <c r="B3" t="n">
-        <v>10462.2</v>
+        <v>14223.3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44942</v>
+        <v>45306</v>
       </c>
       <c r="B4" t="n">
-        <v>10530.8</v>
+        <v>14086.3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44949</v>
+        <v>45313</v>
       </c>
       <c r="B5" t="n">
-        <v>10580</v>
+        <v>14329.2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44956</v>
+        <v>45320</v>
       </c>
       <c r="B6" t="n">
-        <v>10820</v>
+        <v>14530.8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44963</v>
+        <v>45327</v>
       </c>
       <c r="B7" t="n">
-        <v>10857.8</v>
+        <v>14765.8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44970</v>
+        <v>45334</v>
       </c>
       <c r="B8" t="n">
-        <v>10924.5</v>
+        <v>15369.8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44977</v>
+        <v>45341</v>
       </c>
       <c r="B9" t="n">
-        <v>11246.7</v>
+        <v>16606.7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44984</v>
+        <v>45348</v>
       </c>
       <c r="B10" t="n">
-        <v>11559</v>
+        <v>17217.3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44991</v>
+        <v>45355</v>
       </c>
       <c r="B11" t="n">
-        <v>11867.5</v>
+        <v>17846.3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44998</v>
+        <v>45362</v>
       </c>
       <c r="B12" t="n">
-        <v>11748.3</v>
+        <v>18881.7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45004</v>
+        <v>45369</v>
       </c>
       <c r="B13" t="n">
-        <v>11576.7</v>
+        <v>22421.2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45012</v>
+        <v>45376</v>
       </c>
       <c r="B14" t="n">
-        <v>11691.7</v>
+        <v>26609.7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45019</v>
+        <v>45383</v>
       </c>
       <c r="B15" t="n">
-        <v>11640</v>
+        <v>30037.7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45024</v>
+        <v>45390</v>
       </c>
       <c r="B16" t="n">
-        <v>11858.3</v>
+        <v>32657.7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45026</v>
+        <v>45397</v>
       </c>
       <c r="B17" t="n">
-        <v>11641.7</v>
+        <v>35032.8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45033</v>
+        <v>45404</v>
       </c>
       <c r="B18" t="n">
-        <v>11576.7</v>
+        <v>36444.7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45040</v>
+        <v>45418</v>
       </c>
       <c r="B19" t="n">
-        <v>11618.7</v>
+        <v>28363.83</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45047</v>
+        <v>45425</v>
       </c>
       <c r="B20" t="n">
-        <v>11688.3</v>
+        <v>28908.3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45054</v>
+        <v>45439</v>
       </c>
       <c r="B21" t="n">
-        <v>11858.3</v>
+        <v>25158.3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45061</v>
+        <v>45446</v>
       </c>
       <c r="B22" t="n">
-        <v>11925</v>
+        <v>28234.7</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45068</v>
+        <v>45453</v>
       </c>
       <c r="B23" t="n">
-        <v>12075</v>
+        <v>31491.7</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45075</v>
+        <v>45460</v>
       </c>
       <c r="B24" t="n">
-        <v>12207.5</v>
+        <v>34191.7</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45082</v>
+        <v>45467</v>
       </c>
       <c r="B25" t="n">
-        <v>12187.7</v>
+        <v>32950.7</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45089</v>
+        <v>45474</v>
       </c>
       <c r="B26" t="n">
-        <v>11929.2</v>
+        <v>28029.5</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45096</v>
+        <v>45481</v>
       </c>
       <c r="B27" t="n">
-        <v>11926.5</v>
+        <v>27896.5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45103</v>
+        <v>45488</v>
       </c>
       <c r="B28" t="n">
-        <v>11900.8</v>
+        <v>29218</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45110</v>
+        <v>45495</v>
       </c>
       <c r="B29" t="n">
-        <v>12015</v>
+        <v>29380.8</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45117</v>
+        <v>45502</v>
       </c>
       <c r="B30" t="n">
-        <v>12234.2</v>
+        <v>30001.3</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45124</v>
+        <v>45509</v>
       </c>
       <c r="B31" t="n">
-        <v>12335</v>
+        <v>29737</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45131</v>
+        <v>45516</v>
       </c>
       <c r="B32" t="n">
-        <v>12300</v>
+        <v>30532.5</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45138</v>
+        <v>45523</v>
       </c>
       <c r="B33" t="n">
-        <v>12400</v>
+        <v>28863.7</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45145</v>
+        <v>45530</v>
       </c>
       <c r="B34" t="n">
-        <v>12449.7</v>
+        <v>29505</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45152</v>
+        <v>45537</v>
       </c>
       <c r="B35" t="n">
-        <v>12140</v>
+        <v>31460.8</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45159</v>
+        <v>45544</v>
       </c>
       <c r="B36" t="n">
-        <v>12106.7</v>
+        <v>29681</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45166</v>
+        <v>45551</v>
       </c>
       <c r="B37" t="n">
-        <v>12140.2</v>
+        <v>30525.8</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45173</v>
+        <v>45558</v>
       </c>
       <c r="B38" t="n">
-        <v>12172.5</v>
+        <v>30882.2</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45180</v>
+        <v>45565</v>
       </c>
       <c r="B39" t="n">
-        <v>12462.2</v>
+        <v>31437.7</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45187</v>
+        <v>45572</v>
       </c>
       <c r="B40" t="n">
-        <v>12506.7</v>
+        <v>29845</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45194</v>
+        <v>45579</v>
       </c>
       <c r="B41" t="n">
-        <v>12396.8</v>
+        <v>30178.3</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45201</v>
+        <v>45586</v>
       </c>
       <c r="B42" t="n">
-        <v>12335</v>
+        <v>32445</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>45208</v>
+        <v>45593</v>
       </c>
       <c r="B43" t="n">
-        <v>12449.2</v>
+        <v>29553.7</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>45215</v>
+        <v>45600</v>
       </c>
       <c r="B44" t="n">
-        <v>12613.3</v>
+        <v>31241.3</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>45222</v>
+        <v>45607</v>
       </c>
       <c r="B45" t="n">
-        <v>12889.17</v>
+        <v>30069.2</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>45229</v>
+        <v>45614</v>
       </c>
       <c r="B46" t="n">
-        <v>13166.7</v>
+        <v>31529.2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>45236</v>
+        <v>45621</v>
       </c>
       <c r="B47" t="n">
-        <v>13337.3</v>
+        <v>32570</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>45243</v>
+        <v>45628</v>
       </c>
       <c r="B48" t="n">
-        <v>13531.7</v>
+        <v>32780.7</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>45250</v>
+        <v>45635</v>
       </c>
       <c r="B49" t="n">
-        <v>13657.5</v>
+        <v>32459.7</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>45271</v>
+        <v>45642</v>
       </c>
       <c r="B50" t="n">
-        <v>14161.3</v>
+        <v>33968.3</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>45278</v>
+        <v>45656</v>
       </c>
       <c r="B51" t="n">
-        <v>14261.7</v>
+        <v>34900.8</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>45285</v>
+        <v>45663</v>
       </c>
       <c r="B52" t="n">
-        <v>14271.7</v>
+        <v>34633.5</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>45292</v>
+        <v>45670</v>
       </c>
       <c r="B53" t="n">
-        <v>14271.7</v>
+        <v>34229.2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>45299</v>
+        <v>45677</v>
       </c>
       <c r="B54" t="n">
-        <v>14223.3</v>
+        <v>33817.8</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>45306</v>
+        <v>45684</v>
       </c>
       <c r="B55" t="n">
-        <v>14086.3</v>
+        <v>33831.3</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>45313</v>
+        <v>45691</v>
       </c>
       <c r="B56" t="n">
-        <v>14329.2</v>
+        <v>33611</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>45320</v>
+        <v>45698</v>
       </c>
       <c r="B57" t="n">
-        <v>14530.8</v>
+        <v>31623.5</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>45327</v>
+        <v>45705</v>
       </c>
       <c r="B58" t="n">
-        <v>14765.8</v>
+        <v>30533.7</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>45334</v>
+        <v>45712</v>
       </c>
       <c r="B59" t="n">
-        <v>15369.8</v>
+        <v>28345</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>45341</v>
+        <v>45719</v>
       </c>
       <c r="B60" t="n">
-        <v>16606.7</v>
+        <v>26468.3</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>45348</v>
+        <v>45726</v>
       </c>
       <c r="B61" t="n">
-        <v>17217.3</v>
+        <v>23462.8</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>45355</v>
+        <v>45733</v>
       </c>
       <c r="B62" t="n">
-        <v>17846.3</v>
+        <v>22958.2</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>45362</v>
+        <v>45740</v>
       </c>
       <c r="B63" t="n">
-        <v>18881.7</v>
+        <v>23730.8</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>45369</v>
+        <v>45747</v>
       </c>
       <c r="B64" t="n">
-        <v>22421.2</v>
+        <v>23407.5</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>45376</v>
+        <v>45754</v>
       </c>
       <c r="B65" t="n">
-        <v>26609.7</v>
+        <v>23842.2</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>45383</v>
+        <v>45761</v>
       </c>
       <c r="B66" t="n">
-        <v>30037.7</v>
+        <v>25156</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>45390</v>
+        <v>45768</v>
       </c>
       <c r="B67" t="n">
-        <v>32657.7</v>
+        <v>25759.3</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>45397</v>
+        <v>45775</v>
       </c>
       <c r="B68" t="n">
-        <v>35032.8</v>
+        <v>27686.7</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>45404</v>
+        <v>45782</v>
       </c>
       <c r="B69" t="n">
-        <v>36444.7</v>
+        <v>27484.2</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>45418</v>
+        <v>45789</v>
       </c>
       <c r="B70" t="n">
-        <v>28363.83</v>
+        <v>28050.8</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>45425</v>
+        <v>45796</v>
       </c>
       <c r="B71" t="n">
-        <v>28908.3</v>
+        <v>30397</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>45439</v>
+        <v>45803</v>
       </c>
       <c r="B72" t="n">
-        <v>25158.3</v>
+        <v>31486.5</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>45446</v>
+        <v>45810</v>
       </c>
       <c r="B73" t="n">
-        <v>28234.7</v>
+        <v>27863.5</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>45453</v>
+        <v>45817</v>
       </c>
       <c r="B74" t="n">
-        <v>31491.7</v>
+        <v>28895</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>45460</v>
+        <v>45824</v>
       </c>
       <c r="B75" t="n">
-        <v>34191.7</v>
+        <v>30554.5</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>45467</v>
+        <v>45831</v>
       </c>
       <c r="B76" t="n">
-        <v>32950.7</v>
+        <v>28000.8</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>45474</v>
+        <v>45838</v>
       </c>
       <c r="B77" t="n">
-        <v>28029.5</v>
+        <v>27960.7</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>45481</v>
+        <v>45845</v>
       </c>
       <c r="B78" t="n">
-        <v>27896.5</v>
+        <v>25977.5</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
-        <v>45488</v>
+        <v>45852</v>
       </c>
       <c r="B79" t="n">
-        <v>29218</v>
+        <v>25323</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>45495</v>
+        <v>45866</v>
       </c>
       <c r="B80" t="n">
-        <v>29380.8</v>
+        <v>23747</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>45502</v>
+        <v>45873</v>
       </c>
       <c r="B81" t="n">
-        <v>30001.3</v>
+        <v>24127.2</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
-        <v>45509</v>
+        <v>45880</v>
       </c>
       <c r="B82" t="n">
-        <v>29737</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="2" t="n">
-        <v>45516</v>
-      </c>
-      <c r="B83" t="n">
-        <v>30532.5</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="2" t="n">
-        <v>45523</v>
-      </c>
-      <c r="B84" t="n">
-        <v>28863.7</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="2" t="n">
-        <v>45530</v>
-      </c>
-      <c r="B85" t="n">
-        <v>29505</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="2" t="n">
-        <v>45537</v>
-      </c>
-      <c r="B86" t="n">
-        <v>31460.8</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="2" t="n">
-        <v>45544</v>
-      </c>
-      <c r="B87" t="n">
-        <v>29681</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="2" t="n">
-        <v>45551</v>
-      </c>
-      <c r="B88" t="n">
-        <v>30525.8</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="2" t="n">
-        <v>45558</v>
-      </c>
-      <c r="B89" t="n">
-        <v>30882.2</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="2" t="n">
-        <v>45565</v>
-      </c>
-      <c r="B90" t="n">
-        <v>31437.7</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="2" t="n">
-        <v>45572</v>
-      </c>
-      <c r="B91" t="n">
-        <v>29845</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="2" t="n">
-        <v>45579</v>
-      </c>
-      <c r="B92" t="n">
-        <v>30178.3</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="2" t="n">
-        <v>45586</v>
-      </c>
-      <c r="B93" t="n">
-        <v>32445</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="2" t="n">
-        <v>45593</v>
-      </c>
-      <c r="B94" t="n">
-        <v>29553.7</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="2" t="n">
-        <v>45600</v>
-      </c>
-      <c r="B95" t="n">
-        <v>31241.3</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="2" t="n">
-        <v>45607</v>
-      </c>
-      <c r="B96" t="n">
-        <v>30069.2</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="2" t="n">
-        <v>45614</v>
-      </c>
-      <c r="B97" t="n">
-        <v>31529.2</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="2" t="n">
-        <v>45621</v>
-      </c>
-      <c r="B98" t="n">
-        <v>32570</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="2" t="n">
-        <v>45628</v>
-      </c>
-      <c r="B99" t="n">
-        <v>32780.7</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="2" t="n">
-        <v>45635</v>
-      </c>
-      <c r="B100" t="n">
-        <v>32459.7</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="2" t="n">
-        <v>45642</v>
-      </c>
-      <c r="B101" t="n">
-        <v>33968.3</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="2" t="n">
-        <v>45656</v>
-      </c>
-      <c r="B102" t="n">
-        <v>34900.8</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="2" t="n">
-        <v>45663</v>
-      </c>
-      <c r="B103" t="n">
-        <v>34633.5</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="2" t="n">
-        <v>45670</v>
-      </c>
-      <c r="B104" t="n">
-        <v>34229.2</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="2" t="n">
-        <v>45677</v>
-      </c>
-      <c r="B105" t="n">
-        <v>33817.8</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="2" t="n">
-        <v>45684</v>
-      </c>
-      <c r="B106" t="n">
-        <v>33831.3</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="2" t="n">
-        <v>45691</v>
-      </c>
-      <c r="B107" t="n">
-        <v>33611</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="2" t="n">
-        <v>45698</v>
-      </c>
-      <c r="B108" t="n">
-        <v>31623.5</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="2" t="n">
-        <v>45705</v>
-      </c>
-      <c r="B109" t="n">
-        <v>30533.7</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="2" t="n">
-        <v>45712</v>
-      </c>
-      <c r="B110" t="n">
-        <v>28345</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="2" t="n">
-        <v>45719</v>
-      </c>
-      <c r="B111" t="n">
-        <v>26468.3</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="2" t="n">
-        <v>45726</v>
-      </c>
-      <c r="B112" t="n">
-        <v>23462.8</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="2" t="n">
-        <v>45733</v>
-      </c>
-      <c r="B113" t="n">
-        <v>22958.2</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="2" t="n">
-        <v>45740</v>
-      </c>
-      <c r="B114" t="n">
-        <v>23730.8</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="2" t="n">
-        <v>45747</v>
-      </c>
-      <c r="B115" t="n">
-        <v>23407.5</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="2" t="n">
-        <v>45754</v>
-      </c>
-      <c r="B116" t="n">
-        <v>23842.2</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="2" t="n">
-        <v>45761</v>
-      </c>
-      <c r="B117" t="n">
-        <v>25156</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="2" t="n">
-        <v>45768</v>
-      </c>
-      <c r="B118" t="n">
-        <v>25759.3</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" s="2" t="n">
-        <v>45775</v>
-      </c>
-      <c r="B119" t="n">
-        <v>27686.7</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="2" t="n">
-        <v>45782</v>
-      </c>
-      <c r="B120" t="n">
-        <v>27484.2</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="2" t="n">
-        <v>45789</v>
-      </c>
-      <c r="B121" t="n">
-        <v>28050.8</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" s="2" t="n">
-        <v>45796</v>
-      </c>
-      <c r="B122" t="n">
-        <v>30397</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" s="2" t="n">
-        <v>45803</v>
-      </c>
-      <c r="B123" t="n">
-        <v>31486.5</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" s="2" t="n">
-        <v>45810</v>
-      </c>
-      <c r="B124" t="n">
-        <v>27863.5</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" s="2" t="n">
-        <v>45817</v>
-      </c>
-      <c r="B125" t="n">
-        <v>28895</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" s="2" t="n">
-        <v>45824</v>
-      </c>
-      <c r="B126" t="n">
-        <v>30554.5</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" s="2" t="n">
-        <v>45831</v>
-      </c>
-      <c r="B127" t="n">
-        <v>28000.8</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" s="2" t="n">
-        <v>45838</v>
-      </c>
-      <c r="B128" t="n">
-        <v>27960.7</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" s="2" t="n">
-        <v>45845</v>
-      </c>
-      <c r="B129" t="n">
-        <v>25977.5</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="2" t="n">
-        <v>45852</v>
-      </c>
-      <c r="B130" t="n">
-        <v>25323</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" s="2" t="n">
-        <v>45866</v>
-      </c>
-      <c r="B131" t="n">
-        <v>23747</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" s="2" t="n">
-        <v>45873</v>
-      </c>
-      <c r="B132" t="n">
-        <v>24127.2</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" s="2" t="n">
-        <v>45880</v>
-      </c>
-      <c r="B133" t="n">
         <v>24793.8</v>
       </c>
     </row>

</xml_diff>